<commit_message>
Mọi người cố gắng hoàn thiện nhanh nhé!!!
Cố gắng hoàn thiện các nhiệm vụ tớ giao nhé ;))
</commit_message>
<xml_diff>
--- a/Thực tập nhóm.xlsx
+++ b/Thực tập nhóm.xlsx
@@ -54,21 +54,9 @@
     <t>9h-10h</t>
   </si>
   <si>
-    <t>Xây dựng module thêm nhân sự mới</t>
-  </si>
-  <si>
     <t>10h-11h</t>
   </si>
   <si>
-    <t>Xây dựng module sửa nhân sự</t>
-  </si>
-  <si>
-    <t>Xây dựng module xóa nhân sự</t>
-  </si>
-  <si>
-    <t>Xây dựng module tìm kiếm nhân sự</t>
-  </si>
-  <si>
     <t>Xây dựng module hướng dẫn sử dụng phần mềm (menu Help, F1) chi tiết đến từng chức năng</t>
   </si>
   <si>
@@ -106,6 +94,18 @@
   </si>
   <si>
     <t>1,10</t>
+  </si>
+  <si>
+    <t>Xây dựng module sửa nhân sự và phòng ban</t>
+  </si>
+  <si>
+    <t>Xây dựng module xóa nhân sự và phòng ban</t>
+  </si>
+  <si>
+    <t>Xây dựng module tìm kiếm nhân sự và phòng ban</t>
+  </si>
+  <si>
+    <t>Xây dựng module thêm nhân sự và pb mới</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +571,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>8</v>
@@ -587,7 +587,7 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>10</v>
@@ -599,14 +599,14 @@
         <v>1.3</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -615,14 +615,14 @@
         <v>1.4</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -631,30 +631,30 @@
         <v>1.5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="2">
         <v>1.6</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -663,14 +663,14 @@
         <v>1.7</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -679,14 +679,14 @@
         <v>1.8</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -695,30 +695,30 @@
         <v>1.9</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>